<commit_message>
Added CSS selectors to games dictionaries.
</commit_message>
<xml_diff>
--- a/medal-list.xlsx
+++ b/medal-list.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="missing" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -235,7 +236,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -252,4 +253,30 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed scope of workbook variable.
</commit_message>
<xml_diff>
--- a/medal-list.xlsx
+++ b/medal-list.xlsx
@@ -24,13 +24,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0%"/>
+    <numFmt numFmtId="165" formatCode="[$-409]_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="[$-409]_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]_(\$* #,##0_);_(\$* \(#,##0\);_(\$* \-_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="[$-409]_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="[$-409]_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="[$-409]_(\$* #,##0_);_(\$* \(#,##0\);_(\$* \-_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -51,6 +51,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -61,20 +67,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -122,71 +115,71 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -268,15 +261,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test of script proves successful.
</commit_message>
<xml_diff>
--- a/medal-list.xlsx
+++ b/medal-list.xlsx
@@ -4,11 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="missing" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="halo3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
@@ -18,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -46,21 +47,6 @@
       <family val="0"/>
       <sz val="10"/>
     </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="24"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="18"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -112,7 +98,7 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -122,6 +108,7 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -440,17 +427,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H26" activeCellId="0" pane="topLeft" sqref="H26"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="2" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row customHeight="1" ht="12.8" r="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>completed games</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>halo3</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.025" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.025"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="1" verticalDpi="300"/>
@@ -473,11 +475,11 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="1025" min="1" style="2" width="11.52"/>
   </cols>
@@ -494,4 +496,142 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>file name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>medal name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>requirement</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Snap25.png</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Headshot</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Fatally headshot an enemy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Snap24.png</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Multi Kill</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Score three or more kills within 1.5 seconds.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Snap27.png</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Super Detonation</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Load an enemy with at least 7 Needler rounds, causing them to explode.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Snap28.png</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>EMP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Drain an enemy's shields with the Plasma Pistol, Power Drain, or a Plasma Grenade, and then kill them.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Roadkill_Medal.gif</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Splatter</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ram and kill an enemy with a vehicle.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Assassin_Medal.gif</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Assassin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Kill an enemy with a melee attack from behind.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added timer to report how long the scrape took.
</commit_message>
<xml_diff>
--- a/medal-list.xlsx
+++ b/medal-list.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="missing" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -245,30 +244,4 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>